<commit_message>
add first versions of:
cmip6_cccma_citations.xlsx
cmip6/models/canesm5/cmip6_cccma_canesm5_aerosol.xlsx
cmip6/models/canesm5/cmip6_cccma_canesm5_atmos.xlsx
cmip6/models/canesm5/cmip6_cccma_canesm5_atmoschem.xlsx
cmip6/models/canesm5/cmip6_cccma_canesm5_coupling.xlsx
cmip6/models/canesm5/cmip6_cccma_canesm5_toplevel.xlsx
</commit_message>
<xml_diff>
--- a/cmip6/citations/cmip6_cccma_citations.xlsx
+++ b/cmip6/citations/cmip6_cccma_citations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipsl/Engineering/esdoc/bash/cmip6/citations/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ES-DOC\spreadsheet_copies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3B9249-E2A6-2448-9F22-74A155B1A05C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="945" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>ES-DOC CMIP6 Model Citations</t>
   </si>
@@ -81,12 +80,92 @@
   <si>
     <t>Long name for internal use (unarchived)</t>
   </si>
+  <si>
+    <t>Scinocca_et_al_2008</t>
+  </si>
+  <si>
+    <t>10.5194/acp-8-7055-2008</t>
+  </si>
+  <si>
+    <t>von_Salzen_et_al_2013</t>
+  </si>
+  <si>
+    <t>10.1080/07055900.2012.755610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1080/07055900.1995.9649539
+</t>
+  </si>
+  <si>
+    <t>Zhang_McFarlane_1995</t>
+  </si>
+  <si>
+    <t>Scinocca_McFarlane_2004</t>
+  </si>
+  <si>
+    <t>10.1175/1520-0469(2004)061&lt;1993:TVOMTP&gt;2.0.CO;2</t>
+  </si>
+  <si>
+    <t>von_Salzen_McFarlane_2002</t>
+  </si>
+  <si>
+    <t>10.1007/BF00207939</t>
+  </si>
+  <si>
+    <t>10.1175/1520-0469(2002)059&lt;1405:POTBEO&gt;2.0.CO;2</t>
+  </si>
+  <si>
+    <t>Lohmann_Roeckner_1996</t>
+  </si>
+  <si>
+    <t>10.1002/qj.49712656914</t>
+  </si>
+  <si>
+    <t>Hogan_Illingworth_2000</t>
+  </si>
+  <si>
+    <t>Scinocca_McFarlane_2000</t>
+  </si>
+  <si>
+    <t>10.1002/qj.49712656802</t>
+  </si>
+  <si>
+    <t>10.1175/1520-0469(1987)044&lt;1775:TEOOEG&gt;2.0.CO;2</t>
+  </si>
+  <si>
+    <t>McFarlane_1987</t>
+  </si>
+  <si>
+    <t>Arora_Boer_1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1029/1999JD900905
+</t>
+  </si>
+  <si>
+    <t>Lohmann_et_al_1999</t>
+  </si>
+  <si>
+    <t>10.1029/1999JD900343</t>
+  </si>
+  <si>
+    <t>Croft_et_al_2005</t>
+  </si>
+  <si>
+    <t>10.5194/acp-5-1931-2005</t>
+  </si>
+  <si>
+    <t>Lana_et_al_2010</t>
+  </si>
+  <si>
+    <t>10.1029/2010GB003850</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1532,20 +1611,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.1640625" style="1" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="1" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="34.35" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1554,14 +1635,14 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="25.5" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1572,14 +1653,14 @@
       <c r="D3" s="6"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="25.5" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -1590,14 +1671,14 @@
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="408.95" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="408.95" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1606,7 +1687,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1617,7 +1698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1625,17 +1706,17 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="81.83203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="42.83203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="18" customWidth="1"/>
-    <col min="6" max="250" width="16.33203125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="18" customWidth="1"/>
+    <col min="6" max="250" width="16.28515625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:250" ht="30.95" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1725,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="20.85" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -1661,7 +1742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:250" s="27" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:250" s="27" customFormat="1" ht="129" customHeight="1">
       <c r="A3" s="24" t="s">
         <v>13</v>
       </c>
@@ -1921,371 +2002,371 @@
       <c r="IO3" s="26"/>
       <c r="IP3" s="26"/>
     </row>
-    <row r="4" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="23"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="23"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="16"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="16"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="22"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="17"/>
       <c r="B28" s="14"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
     </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="17"/>
       <c r="B29" s="14"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
     </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="17"/>
       <c r="B51" s="22"/>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="17"/>
       <c r="B52" s="22"/>
       <c r="C52" s="22"/>
       <c r="D52" s="22"/>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="17"/>
       <c r="B53" s="22"/>
       <c r="C53" s="22"/>
       <c r="D53" s="22"/>
       <c r="E53" s="22"/>
     </row>
-    <row r="54" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="17"/>
       <c r="B54" s="22"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="17"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
     </row>
-    <row r="56" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="17"/>
       <c r="B56" s="22"/>
       <c r="C56" s="22"/>
@@ -2302,25 +2383,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IP52"/>
+  <dimension ref="A1:IP50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="81.83203125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="42.83203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" style="18" customWidth="1"/>
-    <col min="6" max="250" width="16.33203125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="46.85546875" style="18" customWidth="1"/>
+    <col min="6" max="250" width="16.28515625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:250" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:250" ht="30.95" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -2329,7 +2412,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:250" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:250" ht="20.85" customHeight="1">
       <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
@@ -2352,355 +2435,393 @@
       <c r="IO2"/>
       <c r="IP2"/>
     </row>
-    <row r="3" spans="1:250" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
+    <row r="3" spans="1:250" ht="20.25" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
     </row>
-    <row r="4" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
+    <row r="4" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
     </row>
-    <row r="5" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
+    <row r="5" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
+    <row r="6" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
-    <row r="7" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
+    <row r="7" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
     </row>
-    <row r="8" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
+    <row r="8" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
     </row>
-    <row r="9" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
+    <row r="9" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
+    <row r="10" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="C10" s="16"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
+    <row r="11" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
+    <row r="12" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
+    <row r="13" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
+    <row r="14" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="16"/>
+    <row r="15" spans="1:250" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
     </row>
-    <row r="16" spans="1:250" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:250" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
     </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
     </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="17"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="17"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
     </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
     </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="17"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
     </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="17"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
     </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="17"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="17"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="17"/>
       <c r="B30" s="22"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="17"/>
       <c r="B31" s="22"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="17"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
     </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="17"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
       <c r="D34" s="22"/>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="17"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
     </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="17"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
     </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
       <c r="D38" s="22"/>
       <c r="E38" s="22"/>
     </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
       <c r="E39" s="22"/>
     </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
       <c r="D41" s="22"/>
       <c r="E41" s="22"/>
     </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
       <c r="D42" s="22"/>
       <c r="E42" s="22"/>
     </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="17"/>
       <c r="B49" s="22"/>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="17"/>
       <c r="B50" s="22"/>
       <c r="C50" s="22"/>
       <c r="D50" s="22"/>
       <c r="E50" s="22"/>
-    </row>
-    <row r="51" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="17"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-    </row>
-    <row r="52" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="17"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>